<commit_message>
Update .gitignore to exclude properties files and modify original passwords spreadsheet
</commit_message>
<xml_diff>
--- a/passwords/original_passwords.xlsx
+++ b/passwords/original_passwords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2401606\Downloads\Final Project\Velocity-Vehicles_DB\passwords\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2401604\Downloads\final project\Velocity-Vehicles_DB\passwords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952003AF-69FA-4DD5-A273-E73C62A3B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92408197-112F-43BC-B3AF-FC425F66171C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -760,7 +760,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,7 +789,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1204,6 +1204,7 @@
     <hyperlink ref="D4" r:id="rId11" xr:uid="{585DE8C7-CF0E-40D8-AF15-241507ED0BFB}"/>
     <hyperlink ref="D30" r:id="rId12" xr:uid="{63666EFD-452A-40D5-AF9E-B7D6B522EEF1}"/>
     <hyperlink ref="D7" r:id="rId13" xr:uid="{2BA6D8E8-F067-47F8-8788-75C16E146C8A}"/>
+    <hyperlink ref="B2" r:id="rId14" xr:uid="{E3E018D1-4366-4364-85C0-1965E4B4FBD9}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed the bycript script
</commit_message>
<xml_diff>
--- a/passwords/original_passwords.xlsx
+++ b/passwords/original_passwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2401606\Downloads\Final Project\Velocity-Vehicles_DB\passwords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952003AF-69FA-4DD5-A273-E73C62A3B295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57278F35-1BCE-4C55-9204-E0848BAB5AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,9 +442,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -453,6 +450,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,17 +771,17 @@
     <col min="4" max="4" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -795,7 +795,7 @@
       <c r="C2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>87</v>
       </c>
     </row>
@@ -809,7 +809,7 @@
       <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -893,7 +893,7 @@
       <c r="C9" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       <c r="C17" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1204,6 +1204,10 @@
     <hyperlink ref="D4" r:id="rId11" xr:uid="{585DE8C7-CF0E-40D8-AF15-241507ED0BFB}"/>
     <hyperlink ref="D30" r:id="rId12" xr:uid="{63666EFD-452A-40D5-AF9E-B7D6B522EEF1}"/>
     <hyperlink ref="D7" r:id="rId13" xr:uid="{2BA6D8E8-F067-47F8-8788-75C16E146C8A}"/>
+    <hyperlink ref="D2" r:id="rId14" xr:uid="{3C1B5CE6-CB6F-4F72-BD28-F2759670BAFD}"/>
+    <hyperlink ref="D3" r:id="rId15" xr:uid="{812715AB-2411-4B8B-AAB7-99464A365045}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{9F5E92D0-067F-4407-8A91-9C646BD005CF}"/>
+    <hyperlink ref="D9" r:id="rId17" xr:uid="{0FDFD2B0-2BB4-4FE6-B1FF-5FEE1AC20960}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update database configuration and remove original passwords file
</commit_message>
<xml_diff>
--- a/passwords/original_passwords.xlsx
+++ b/passwords/original_passwords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2401606\Downloads\Final Project\Velocity-Vehicles_DB\passwords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520BE629-A4CA-4D83-9C00-41773B9B6D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B11358-DBC1-4A5B-A365-16C10B486E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Password Audit" sheetId="1" r:id="rId1"/>
@@ -760,7 +760,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -803,7 +803,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
@@ -1212,6 +1212,7 @@
     <hyperlink ref="B8" r:id="rId19" xr:uid="{0EBB89EF-A070-4ACF-8A1D-056736F3EF27}"/>
     <hyperlink ref="D23" r:id="rId20" xr:uid="{F1BDA9DF-7BBF-4468-9ED9-9450AF84B070}"/>
     <hyperlink ref="B7" r:id="rId21" xr:uid="{0361EDB6-E7A0-4B0B-99D0-AA79ED858963}"/>
+    <hyperlink ref="B3" r:id="rId22" xr:uid="{B46D5C58-9B53-4C6A-9398-61268F60BF85}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>